<commit_message>
Second iteration. Add analizing system determination of whole portfolio based. All through LLM. Updated OCR system with more clear scaning
</commit_message>
<xml_diff>
--- a/data/output/report.xlsx
+++ b/data/output/report.xlsx
@@ -483,7 +483,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Присвоена степень бакалавра по направлению Информатика и Вычислительная Техника, с присвоением специального звания "Бакалавр-Инженер".</t>
+          <t>Это приложение к диплому, где указывается специальность и степень, которую получает студент (в данном случае - бакалавр-инженер в области Информатики и Вычислительная Техника).</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -510,22 +510,22 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Документ, удостоверяющий получение степени бакалавра в области Информатики и Вычислительная Техника</t>
+          <t>Диплом бакалавра</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Данный документ является дипломом бакалавра по специальности 230100 - Информатика и Вычислительная Техника, с присвоением ему специального звания.</t>
+          <t>Этот документ присвоен степени бакалавра и содержит сведения о личности обладателя диплома, ученом звании, специальности, дате рождения, предыдущем уровне образования и названию и адресу учебного заведения.</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>0.14</t>
+          <t>1.00</t>
         </is>
       </c>
     </row>
@@ -542,18 +542,22 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Описание</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
+          <t>Приложение к диплому</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Содержит список дисциплин (модулей) основной образовательной программы в высшем профессиональном учебном заведении.</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>❌</t>
+          <t>✅</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>1.00</t>
         </is>
       </c>
     </row>
@@ -575,7 +579,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Имя и номер теста указываются, также как срок действия сертификата и адрес веб-сайта для проверки.</t>
+          <t>Этот документ подтверждает результаты теста по английскому языку (IELTS), который был проведён для определения способности кандидата к обучению на английском языке.</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">

</xml_diff>